<commit_message>
Fix Dragon Blood Potion + OAAB Grazelands
</commit_message>
<xml_diff>
--- a/BetterNames-v2.1-Alchemy.xlsx
+++ b/BetterNames-v2.1-Alchemy.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7425" uniqueCount="1482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7459" uniqueCount="1491">
   <si>
     <t>ALCH</t>
   </si>
@@ -4476,6 +4476,33 @@
   </si>
   <si>
     <t>Bottle of Absinthe</t>
+  </si>
+  <si>
+    <t>Potion of Dragon's Blood</t>
+  </si>
+  <si>
+    <t>ABtv_pot_CureParalysis</t>
+  </si>
+  <si>
+    <t>Aryon's Cure for Paralyzation</t>
+  </si>
+  <si>
+    <t>Cure Paralysis by Aryon</t>
+  </si>
+  <si>
+    <t>Potion Cure Paralysis by Aryon</t>
+  </si>
+  <si>
+    <t>ABtv_pot_CureBlightMMCure</t>
+  </si>
+  <si>
+    <t>ABtv_dri_SheinVintage</t>
+  </si>
+  <si>
+    <t>Vintage Wine</t>
+  </si>
+  <si>
+    <t>Bottle of Vintage Wine</t>
   </si>
 </sst>
 </file>
@@ -13722,10 +13749,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N367"/>
+  <dimension ref="A1:N369"/>
   <sheetViews>
-    <sheetView topLeftCell="A333" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I367"/>
+    <sheetView topLeftCell="A343" workbookViewId="0">
+      <selection activeCell="A367" sqref="A367:A369"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24724,14 +24751,14 @@
         <v>941</v>
       </c>
       <c r="H322">
-        <f t="shared" ref="H322:H367" si="10">LEN(G322)</f>
+        <f t="shared" ref="H322:H369" si="10">LEN(G322)</f>
         <v>20</v>
       </c>
       <c r="I322" t="s">
         <v>1057</v>
       </c>
       <c r="J322">
-        <f t="shared" ref="J322:J367" si="11">LEN(I322)</f>
+        <f t="shared" ref="J322:J369" si="11">LEN(I322)</f>
         <v>27</v>
       </c>
     </row>
@@ -26263,6 +26290,74 @@
       <c r="J367">
         <f t="shared" si="11"/>
         <v>24</v>
+      </c>
+    </row>
+    <row r="368" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A368" t="s">
+        <v>875</v>
+      </c>
+      <c r="B368" t="s">
+        <v>1483</v>
+      </c>
+      <c r="C368" t="s">
+        <v>1484</v>
+      </c>
+      <c r="D368" s="2">
+        <v>0</v>
+      </c>
+      <c r="E368" s="2">
+        <v>0</v>
+      </c>
+      <c r="F368" s="2">
+        <v>0</v>
+      </c>
+      <c r="G368" s="2" t="s">
+        <v>1485</v>
+      </c>
+      <c r="H368">
+        <f t="shared" si="10"/>
+        <v>23</v>
+      </c>
+      <c r="I368" s="2" t="s">
+        <v>1486</v>
+      </c>
+      <c r="J368">
+        <f t="shared" si="11"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="369" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A369" t="s">
+        <v>875</v>
+      </c>
+      <c r="B369" t="s">
+        <v>1487</v>
+      </c>
+      <c r="C369" t="s">
+        <v>437</v>
+      </c>
+      <c r="D369" s="2">
+        <v>0</v>
+      </c>
+      <c r="E369" s="2">
+        <v>0</v>
+      </c>
+      <c r="F369" s="2">
+        <v>0</v>
+      </c>
+      <c r="G369" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="H369">
+        <f t="shared" si="10"/>
+        <v>19</v>
+      </c>
+      <c r="I369" s="2" t="s">
+        <v>1032</v>
+      </c>
+      <c r="J369">
+        <f t="shared" si="11"/>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -26283,9 +26378,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:D471"/>
+  <dimension ref="A1:D474"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A434" workbookViewId="0">
+      <selection activeCell="D472" sqref="D472:D474"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -32919,7 +33016,7 @@
         <v>1474</v>
       </c>
       <c r="D442" t="str">
-        <f t="shared" ref="D442:D471" si="7">IF(B442&lt;&gt;C442,"{ID="&amp;""""&amp;A442&amp;""""&amp;", name="&amp;""""&amp;C442&amp;""""&amp;"},","")</f>
+        <f t="shared" ref="D442:D474" si="7">IF(B442&lt;&gt;C442,"{ID="&amp;""""&amp;A442&amp;""""&amp;", name="&amp;""""&amp;C442&amp;""""&amp;"},","")</f>
         <v>{ID="Ascadian Ale4", name="Mug of Dead Guard"},</v>
       </c>
     </row>
@@ -33356,6 +33453,51 @@
       <c r="D471" t="str">
         <f t="shared" si="7"/>
         <v>{ID="MI_absinthe", name="Bottle of Absinthe"},</v>
+      </c>
+    </row>
+    <row r="472" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A472" t="s">
+        <v>1483</v>
+      </c>
+      <c r="B472" t="s">
+        <v>1484</v>
+      </c>
+      <c r="C472" s="2" t="s">
+        <v>1485</v>
+      </c>
+      <c r="D472" t="str">
+        <f t="shared" si="7"/>
+        <v>{ID="ABtv_pot_CureParalysis", name="Cure Paralysis by Aryon"},</v>
+      </c>
+    </row>
+    <row r="473" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A473" t="s">
+        <v>1487</v>
+      </c>
+      <c r="B473" t="s">
+        <v>437</v>
+      </c>
+      <c r="C473" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="D473" t="str">
+        <f t="shared" si="7"/>
+        <v>{ID="ABtv_pot_CureBlightMMCure", name="Cure Blight Disease"},</v>
+      </c>
+    </row>
+    <row r="474" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A474" t="s">
+        <v>1488</v>
+      </c>
+      <c r="B474" t="s">
+        <v>1489</v>
+      </c>
+      <c r="C474" t="s">
+        <v>1490</v>
+      </c>
+      <c r="D474" t="str">
+        <f t="shared" si="7"/>
+        <v>{ID="ABtv_dri_SheinVintage", name="Bottle of Vintage Wine"},</v>
       </c>
     </row>
   </sheetData>
@@ -33373,9 +33515,11 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:D471"/>
+  <dimension ref="A1:D474"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A440" workbookViewId="0">
+      <selection activeCell="A475" sqref="A475"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -40144,7 +40288,7 @@
         <v>822</v>
       </c>
       <c r="D451" t="str">
-        <f t="shared" ref="D451:D471" si="7">IF(B451&lt;&gt;C451,"{ID="&amp;""""&amp;A451&amp;""""&amp;", name="&amp;""""&amp;C451&amp;""""&amp;"},","")</f>
+        <f t="shared" ref="D451:D474" si="7">IF(B451&lt;&gt;C451,"{ID="&amp;""""&amp;A451&amp;""""&amp;", name="&amp;""""&amp;C451&amp;""""&amp;"},","")</f>
         <v/>
       </c>
     </row>
@@ -40446,6 +40590,51 @@
       <c r="D471" t="str">
         <f t="shared" si="7"/>
         <v>{ID="MI_absinthe", name="Bottle of Absinthe"},</v>
+      </c>
+    </row>
+    <row r="472" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A472" t="s">
+        <v>1483</v>
+      </c>
+      <c r="B472" t="s">
+        <v>1484</v>
+      </c>
+      <c r="C472" s="2" t="s">
+        <v>1486</v>
+      </c>
+      <c r="D472" t="str">
+        <f t="shared" si="7"/>
+        <v>{ID="ABtv_pot_CureParalysis", name="Potion Cure Paralysis by Aryon"},</v>
+      </c>
+    </row>
+    <row r="473" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A473" t="s">
+        <v>1487</v>
+      </c>
+      <c r="B473" t="s">
+        <v>437</v>
+      </c>
+      <c r="C473" s="2" t="s">
+        <v>1032</v>
+      </c>
+      <c r="D473" t="str">
+        <f t="shared" si="7"/>
+        <v>{ID="ABtv_pot_CureBlightMMCure", name="Potion Cure Blight Disease"},</v>
+      </c>
+    </row>
+    <row r="474" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A474" t="s">
+        <v>1488</v>
+      </c>
+      <c r="B474" t="s">
+        <v>1489</v>
+      </c>
+      <c r="C474" t="s">
+        <v>1490</v>
+      </c>
+      <c r="D474" t="str">
+        <f t="shared" si="7"/>
+        <v>{ID="ABtv_dri_SheinVintage", name="Bottle of Vintage Wine"},</v>
       </c>
     </row>
   </sheetData>
@@ -40463,10 +40652,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J481"/>
+  <dimension ref="A1:J482"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I465" sqref="I465"/>
+    <sheetView topLeftCell="A437" workbookViewId="0">
+      <selection activeCell="I482" sqref="I482"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50444,7 +50633,7 @@
         <v>#N/A</v>
       </c>
       <c r="H400" t="str">
-        <f t="shared" ref="H400:H409" si="11">"Bottle of "&amp;C400</f>
+        <f t="shared" ref="H400:H408" si="11">"Bottle of "&amp;C400</f>
         <v>Bottle of Vitriol Oil</v>
       </c>
       <c r="I400">
@@ -50452,7 +50641,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="401" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>0</v>
       </c>
@@ -50484,7 +50673,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="402" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>0</v>
       </c>
@@ -50516,7 +50705,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="403" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>0</v>
       </c>
@@ -50548,7 +50737,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="404" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>0</v>
       </c>
@@ -50580,7 +50769,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="405" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>0</v>
       </c>
@@ -50611,7 +50800,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="406" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>0</v>
       </c>
@@ -50642,7 +50831,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="407" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>0</v>
       </c>
@@ -50674,7 +50863,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="408" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>0</v>
       </c>
@@ -50706,7 +50895,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="409" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>0</v>
       </c>
@@ -50729,16 +50918,18 @@
         <f>VLOOKUP(B409,'Alchemy-ALL-PotionsOnly'!B:B,1,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H409" t="str">
-        <f t="shared" si="11"/>
-        <v>Bottle of Dragon's Blood</v>
+      <c r="H409" t="s">
+        <v>1482</v>
       </c>
       <c r="I409">
         <f t="shared" si="12"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="410" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J409" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="410" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>0</v>
       </c>
@@ -50769,7 +50960,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="411" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>0</v>
       </c>
@@ -50797,7 +50988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="412" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>0</v>
       </c>
@@ -50825,7 +51016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="413" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>0</v>
       </c>
@@ -50853,7 +51044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="414" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>0</v>
       </c>
@@ -50881,7 +51072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="415" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>0</v>
       </c>
@@ -50909,7 +51100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="416" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>0</v>
       </c>
@@ -52302,7 +52493,7 @@
         <v>1387</v>
       </c>
       <c r="I464">
-        <f t="shared" ref="I464:I481" si="20">LEN(H464)</f>
+        <f t="shared" ref="I464:I482" si="20">LEN(H464)</f>
         <v>23</v>
       </c>
     </row>
@@ -52824,6 +53015,37 @@
       <c r="I481">
         <f t="shared" si="20"/>
         <v>18</v>
+      </c>
+    </row>
+    <row r="482" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A482" t="s">
+        <v>0</v>
+      </c>
+      <c r="B482" t="s">
+        <v>1488</v>
+      </c>
+      <c r="C482" t="s">
+        <v>1489</v>
+      </c>
+      <c r="D482">
+        <v>0</v>
+      </c>
+      <c r="E482">
+        <v>0</v>
+      </c>
+      <c r="F482">
+        <v>0</v>
+      </c>
+      <c r="G482" t="e">
+        <f>VLOOKUP(B482,'Alchemy-ALL-PotionsOnly'!B:B,1,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H482" t="s">
+        <v>1490</v>
+      </c>
+      <c r="I482">
+        <f t="shared" si="20"/>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>